<commit_message>
Single Entity Routing Complete
</commit_message>
<xml_diff>
--- a/intents.xlsx
+++ b/intents.xlsx
@@ -4293,8 +4293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9930,6 +9930,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1"/>
   <hyperlinks>
     <hyperlink ref="D160" r:id="rId1"/>
     <hyperlink ref="D154" r:id="rId2" display="https://indianvisaonline.gov.in/visa/index.html"/>

</xml_diff>

<commit_message>
Updating Single Entity Routing
</commit_message>
<xml_diff>
--- a/intents.xlsx
+++ b/intents.xlsx
@@ -4293,8 +4293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>